<commit_message>
working version except that the number of topics of each reviewer is still not reflected on number of days
</commit_message>
<xml_diff>
--- a/sample_bachelor_topics.xlsx
+++ b/sample_bachelor_topics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8610590cbf95aee3/Desktop/Darsh/thesis-scheduler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{BCBD197D-9814-4DF4-800F-014CD1E94220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A617FA2-F71E-4884-AC4F-D318AEAD6FF3}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="8_{BCBD197D-9814-4DF4-800F-014CD1E94220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50D0D74A-BBFB-43F3-8AB6-E0B139416556}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{1201BA06-69EF-4164-A6F7-EBA90680A521}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="62">
   <si>
     <t>Title</t>
   </si>
@@ -53,53 +53,182 @@
     <t>Reviewer Email</t>
   </si>
   <si>
-    <t>AI in Medicine</t>
-  </si>
-  <si>
-    <t>Dr. Ahmed</t>
-  </si>
-  <si>
-    <t>ahmed@guc.edu.eg</t>
-  </si>
-  <si>
-    <t>Dr. Mona</t>
-  </si>
-  <si>
-    <t>mona@guc.edu.eg</t>
-  </si>
-  <si>
-    <t>IoT in Agriculture</t>
-  </si>
-  <si>
-    <t>Dr. Rania</t>
-  </si>
-  <si>
-    <t>rania@guc.edu.eg</t>
-  </si>
-  <si>
-    <t>Dr. Hossam</t>
-  </si>
-  <si>
-    <t>hossam@guc.edu.eg</t>
-  </si>
-  <si>
-    <t>Robotics in Surgery</t>
-  </si>
-  <si>
-    <t>AI in Diagnostics</t>
-  </si>
-  <si>
-    <t>Dr. Darsh</t>
-  </si>
-  <si>
-    <t>darsh@guc.edu.eg</t>
+    <t>FT Supervisor 1</t>
+  </si>
+  <si>
+    <t>ft1@example.com</t>
+  </si>
+  <si>
+    <t>Reviewer 1</t>
+  </si>
+  <si>
+    <t>rev1@example.com</t>
+  </si>
+  <si>
+    <t>FT Supervisor 2</t>
+  </si>
+  <si>
+    <t>ft2@example.com</t>
+  </si>
+  <si>
+    <t>Reviewer 2</t>
+  </si>
+  <si>
+    <t>rev2@example.com</t>
+  </si>
+  <si>
+    <t>FT Supervisor 3</t>
+  </si>
+  <si>
+    <t>ft3@example.com</t>
+  </si>
+  <si>
+    <t>Reviewer 3</t>
+  </si>
+  <si>
+    <t>rev3@example.com</t>
+  </si>
+  <si>
+    <t>FT Supervisor 4</t>
+  </si>
+  <si>
+    <t>ft4@example.com</t>
+  </si>
+  <si>
+    <t>Reviewer 4</t>
+  </si>
+  <si>
+    <t>rev4@example.com</t>
+  </si>
+  <si>
+    <t>FT Supervisor 5</t>
+  </si>
+  <si>
+    <t>ft5@example.com</t>
+  </si>
+  <si>
+    <t>Reviewer 5</t>
+  </si>
+  <si>
+    <t>rev5@example.com</t>
+  </si>
+  <si>
+    <t>FT Supervisor 6</t>
+  </si>
+  <si>
+    <t>FT Supervisor 7</t>
+  </si>
+  <si>
+    <t>FT Supervisor 8</t>
+  </si>
+  <si>
+    <t>FT Supervisor 9</t>
+  </si>
+  <si>
+    <t>FT Supervisor 10</t>
+  </si>
+  <si>
+    <t>ft6@example.com</t>
+  </si>
+  <si>
+    <t>ft7@example.com</t>
+  </si>
+  <si>
+    <t>ft8@example.com</t>
+  </si>
+  <si>
+    <t>ft9@example.com</t>
+  </si>
+  <si>
+    <t>ft10@example.com</t>
+  </si>
+  <si>
+    <t>Reviewer 6</t>
+  </si>
+  <si>
+    <t>Reviewer 7</t>
+  </si>
+  <si>
+    <t>Reviewer 8</t>
+  </si>
+  <si>
+    <t>Reviewer 9</t>
+  </si>
+  <si>
+    <t>Reviewer 10</t>
+  </si>
+  <si>
+    <t>rev6@example.com</t>
+  </si>
+  <si>
+    <t>rev7@example.com</t>
+  </si>
+  <si>
+    <t>rev8@example.com</t>
+  </si>
+  <si>
+    <t>rev9@example.com</t>
+  </si>
+  <si>
+    <t>rev10@example.com</t>
+  </si>
+  <si>
+    <t>Topic 2</t>
+  </si>
+  <si>
+    <t>Topic 1</t>
+  </si>
+  <si>
+    <t>Topic 3</t>
+  </si>
+  <si>
+    <t>Topic 4</t>
+  </si>
+  <si>
+    <t>Topic 5</t>
+  </si>
+  <si>
+    <t>Topic 6</t>
+  </si>
+  <si>
+    <t>Topic 7</t>
+  </si>
+  <si>
+    <t>Topic 8</t>
+  </si>
+  <si>
+    <t>Topic 9</t>
+  </si>
+  <si>
+    <t>Topic 10</t>
+  </si>
+  <si>
+    <t>Topic 11</t>
+  </si>
+  <si>
+    <t>Topic 12</t>
+  </si>
+  <si>
+    <t>Topic 13</t>
+  </si>
+  <si>
+    <t>Topic 14</t>
+  </si>
+  <si>
+    <t>Topic 15</t>
+  </si>
+  <si>
+    <t>Topic 16</t>
+  </si>
+  <si>
+    <t>Topic 17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +240,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -143,7 +278,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -153,7 +288,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -495,15 +630,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E079B945-F8AC-458B-99EE-C796BEC86543}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.15625" customWidth="1"/>
     <col min="2" max="2" width="19.734375" customWidth="1"/>
     <col min="3" max="3" width="20.68359375" customWidth="1"/>
     <col min="4" max="4" width="23.5234375" customWidth="1"/>
@@ -529,75 +664,313 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{45B3A98C-C24D-49D1-9039-6F717E8383C5}"/>
+    <hyperlink ref="C7" r:id="rId1" xr:uid="{75EA1003-1BE7-4997-B04B-3CD4FF2B8016}"/>
+    <hyperlink ref="C8" r:id="rId2" xr:uid="{D4E8E1E0-D65F-4F91-9389-17E75AD8C4CF}"/>
+    <hyperlink ref="C9" r:id="rId3" xr:uid="{9E608505-8E1B-48B0-957A-C9D1C01E0DFF}"/>
+    <hyperlink ref="C10" r:id="rId4" xr:uid="{3739452D-1093-4743-A84F-948927466809}"/>
+    <hyperlink ref="C11" r:id="rId5" xr:uid="{70443444-1526-4412-A29A-B555987F1E2F}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{30B68F94-1E0A-41B0-A31B-B1147398B972}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{48E1957A-DB6C-4BF5-995E-3C992F095C62}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{4C6F6A11-6C0A-4BBD-83C4-32D654EC32B7}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{C405A3A0-5F5D-47E0-AEA7-AB9FA77D6784}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{E8F61D55-56C4-420A-8C9C-09D47F475E3A}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{F0F9DD13-BC84-4D4D-AFF8-DA2BB8D57C0E}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{D980B3D8-8536-4EB3-A9BF-B1C1249245E9}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{C084C175-9D1B-47BC-9B69-9A4535AEAFF3}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{33CA14C9-6E4E-46D9-A978-2F1942AFB5F3}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{EEEC920E-76F5-4736-8164-C40A87EABDCD}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{51B883F3-908E-46CF-8F9D-A7159266DB44}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{A2CC73A0-F769-4F10-A0BC-DE4F8E4149BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
final edit to yesterday's talk
</commit_message>
<xml_diff>
--- a/sample_bachelor_topics.xlsx
+++ b/sample_bachelor_topics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8610590cbf95aee3/Desktop/Darsh/thesis-scheduler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="8_{BCBD197D-9814-4DF4-800F-014CD1E94220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50D0D74A-BBFB-43F3-8AB6-E0B139416556}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="8_{BCBD197D-9814-4DF4-800F-014CD1E94220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A1CB4C0-BA92-4EB2-A23C-6F3751D57F8D}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{1201BA06-69EF-4164-A6F7-EBA90680A521}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
   <si>
     <t>Title</t>
   </si>
@@ -71,48 +71,24 @@
     <t>ft2@example.com</t>
   </si>
   <si>
-    <t>Reviewer 2</t>
-  </si>
-  <si>
-    <t>rev2@example.com</t>
-  </si>
-  <si>
     <t>FT Supervisor 3</t>
   </si>
   <si>
     <t>ft3@example.com</t>
   </si>
   <si>
-    <t>Reviewer 3</t>
-  </si>
-  <si>
-    <t>rev3@example.com</t>
-  </si>
-  <si>
     <t>FT Supervisor 4</t>
   </si>
   <si>
     <t>ft4@example.com</t>
   </si>
   <si>
-    <t>Reviewer 4</t>
-  </si>
-  <si>
-    <t>rev4@example.com</t>
-  </si>
-  <si>
     <t>FT Supervisor 5</t>
   </si>
   <si>
     <t>ft5@example.com</t>
   </si>
   <si>
-    <t>Reviewer 5</t>
-  </si>
-  <si>
-    <t>rev5@example.com</t>
-  </si>
-  <si>
     <t>FT Supervisor 6</t>
   </si>
   <si>
@@ -141,36 +117,6 @@
   </si>
   <si>
     <t>ft10@example.com</t>
-  </si>
-  <si>
-    <t>Reviewer 6</t>
-  </si>
-  <si>
-    <t>Reviewer 7</t>
-  </si>
-  <si>
-    <t>Reviewer 8</t>
-  </si>
-  <si>
-    <t>Reviewer 9</t>
-  </si>
-  <si>
-    <t>Reviewer 10</t>
-  </si>
-  <si>
-    <t>rev6@example.com</t>
-  </si>
-  <si>
-    <t>rev7@example.com</t>
-  </si>
-  <si>
-    <t>rev8@example.com</t>
-  </si>
-  <si>
-    <t>rev9@example.com</t>
-  </si>
-  <si>
-    <t>rev10@example.com</t>
   </si>
   <si>
     <t>Topic 2</t>
@@ -633,7 +579,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E2" sqref="E2:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -664,7 +610,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -681,7 +627,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -690,157 +636,157 @@
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>40</v>
+        <v>7</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>41</v>
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>42</v>
+        <v>7</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>43</v>
+        <v>7</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>44</v>
+        <v>7</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>7</v>
@@ -851,13 +797,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>7</v>
@@ -868,13 +814,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>7</v>
@@ -885,13 +831,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>7</v>
@@ -902,13 +848,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>7</v>
@@ -919,13 +865,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>7</v>
@@ -936,13 +882,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>7</v>
@@ -959,18 +905,13 @@
     <hyperlink ref="C9" r:id="rId3" xr:uid="{9E608505-8E1B-48B0-957A-C9D1C01E0DFF}"/>
     <hyperlink ref="C10" r:id="rId4" xr:uid="{3739452D-1093-4743-A84F-948927466809}"/>
     <hyperlink ref="C11" r:id="rId5" xr:uid="{70443444-1526-4412-A29A-B555987F1E2F}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{30B68F94-1E0A-41B0-A31B-B1147398B972}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{48E1957A-DB6C-4BF5-995E-3C992F095C62}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{4C6F6A11-6C0A-4BBD-83C4-32D654EC32B7}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{C405A3A0-5F5D-47E0-AEA7-AB9FA77D6784}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{E8F61D55-56C4-420A-8C9C-09D47F475E3A}"/>
-    <hyperlink ref="C12" r:id="rId11" xr:uid="{F0F9DD13-BC84-4D4D-AFF8-DA2BB8D57C0E}"/>
-    <hyperlink ref="C13" r:id="rId12" xr:uid="{D980B3D8-8536-4EB3-A9BF-B1C1249245E9}"/>
-    <hyperlink ref="C14" r:id="rId13" xr:uid="{C084C175-9D1B-47BC-9B69-9A4535AEAFF3}"/>
-    <hyperlink ref="C15" r:id="rId14" xr:uid="{33CA14C9-6E4E-46D9-A978-2F1942AFB5F3}"/>
-    <hyperlink ref="C16" r:id="rId15" xr:uid="{EEEC920E-76F5-4736-8164-C40A87EABDCD}"/>
-    <hyperlink ref="C17" r:id="rId16" xr:uid="{51B883F3-908E-46CF-8F9D-A7159266DB44}"/>
-    <hyperlink ref="C18" r:id="rId17" xr:uid="{A2CC73A0-F769-4F10-A0BC-DE4F8E4149BB}"/>
+    <hyperlink ref="C12" r:id="rId6" xr:uid="{F0F9DD13-BC84-4D4D-AFF8-DA2BB8D57C0E}"/>
+    <hyperlink ref="C13" r:id="rId7" xr:uid="{D980B3D8-8536-4EB3-A9BF-B1C1249245E9}"/>
+    <hyperlink ref="C14" r:id="rId8" xr:uid="{C084C175-9D1B-47BC-9B69-9A4535AEAFF3}"/>
+    <hyperlink ref="C15" r:id="rId9" xr:uid="{33CA14C9-6E4E-46D9-A978-2F1942AFB5F3}"/>
+    <hyperlink ref="C16" r:id="rId10" xr:uid="{EEEC920E-76F5-4736-8164-C40A87EABDCD}"/>
+    <hyperlink ref="C17" r:id="rId11" xr:uid="{51B883F3-908E-46CF-8F9D-A7159266DB44}"/>
+    <hyperlink ref="C18" r:id="rId12" xr:uid="{A2CC73A0-F769-4F10-A0BC-DE4F8E4149BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>